<commit_message>
Updated testing results in expectedResults.xlsx
</commit_message>
<xml_diff>
--- a/test_data/expectedResults.xlsx
+++ b/test_data/expectedResults.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/Library/CloudStorage/Dropbox/HEA Internal/Sales-Government/CEC/2024 Panel Tool GFO/HEA docs/Test files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/Library/CloudStorage/Dropbox/eJobShop/Jobs/HEA Dev/Cursor/NEC-220.87-Methods/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB3C9ED-01F1-6D4C-8E4C-F8A17733F10F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3922D7C1-DEE8-B849-85EF-8638326CC192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2500" yWindow="10280" windowWidth="23560" windowHeight="17440" xr2:uid="{CE87201A-B42D-0F43-8840-BF0117D2FC47}"/>
+    <workbookView xWindow="4600" yWindow="15960" windowWidth="24760" windowHeight="11360" xr2:uid="{CE87201A-B42D-0F43-8840-BF0117D2FC47}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Test</t>
   </si>
@@ -87,6 +87,12 @@
   </si>
   <si>
     <t>Methods/Implementations:</t>
+  </si>
+  <si>
+    <t>HEA-jupyter</t>
+  </si>
+  <si>
+    <t>[fail]</t>
   </si>
 </sst>
 </file>
@@ -497,41 +503,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCAFCC87-39BA-6245-A224-CE73602DEFB2}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="21.5" customWidth="1"/>
-    <col min="2" max="5" width="9.6640625" style="2" customWidth="1"/>
+    <col min="2" max="6" width="9.6640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="B1" s="6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" s="1" customFormat="1">
+      <c r="C1" s="6"/>
+    </row>
+    <row r="2" spans="1:6" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -541,41 +551,53 @@
       <c r="C3" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="D3" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="3">
-        <v>4.0999999999999996</v>
+        <v>4.09</v>
       </c>
       <c r="C4" s="3">
         <v>4.09</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="D4" s="3">
+        <v>4.09</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="D5" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="3">
-        <v>4.0999999999999996</v>
+        <v>4.09</v>
       </c>
       <c r="C6" s="3">
         <v>4.09</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="D6" s="3">
+        <v>4.09</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -583,10 +605,13 @@
         <v>4.21</v>
       </c>
       <c r="C7" s="3">
+        <v>4.21</v>
+      </c>
+      <c r="D7" s="3">
         <v>4.2</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -596,11 +621,14 @@
       <c r="C8" s="4">
         <v>6.2</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
+        <v>6.2</v>
+      </c>
+      <c r="E8" s="5">
         <v>4.7667000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -610,11 +638,14 @@
       <c r="C9" s="3">
         <v>10.71</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="3">
+        <v>10.71</v>
+      </c>
+      <c r="E9" s="2">
         <v>8.24</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -624,8 +655,11 @@
       <c r="C10" s="3">
         <v>9.4600000000000009</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="D10" s="3">
+        <v>9.4600000000000009</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -635,8 +669,11 @@
       <c r="C11" s="3">
         <v>27.85</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="D11" s="3">
+        <v>27.85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -646,7 +683,10 @@
       <c r="C12" s="3">
         <v>7.95</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="3">
+        <v>7.95</v>
+      </c>
+      <c r="E12" s="5">
         <v>1.9869000000000001</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added two new methods to the calculator: LBNL and NEC. Applies different safety margins to the calculations for hourly readings.
</commit_message>
<xml_diff>
--- a/test_data/expectedResults.xlsx
+++ b/test_data/expectedResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/Library/CloudStorage/Dropbox/eJobShop/Jobs/HEA Dev/Cursor/NEC-220.87-Methods/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3922D7C1-DEE8-B849-85EF-8638326CC192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA48509B-DB06-0141-86FB-D16F34EEC78B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4600" yWindow="15960" windowWidth="24760" windowHeight="11360" xr2:uid="{CE87201A-B42D-0F43-8840-BF0117D2FC47}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>Test</t>
   </si>
@@ -506,7 +506,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -554,6 +554,12 @@
       <c r="D3" s="3">
         <v>5</v>
       </c>
+      <c r="E3" s="2">
+        <v>5</v>
+      </c>
+      <c r="F3" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
@@ -568,6 +574,12 @@
       <c r="D4" s="3">
         <v>4.09</v>
       </c>
+      <c r="E4" s="2">
+        <v>3.15</v>
+      </c>
+      <c r="F4" s="2">
+        <v>6.61</v>
+      </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
@@ -582,6 +594,12 @@
       <c r="D5" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="E5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
@@ -596,6 +614,12 @@
       <c r="D6" s="3">
         <v>4.09</v>
       </c>
+      <c r="E6" s="2">
+        <v>3.4</v>
+      </c>
+      <c r="F6" s="2">
+        <v>6.61</v>
+      </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
@@ -610,6 +634,12 @@
       <c r="D7" s="3">
         <v>4.2</v>
       </c>
+      <c r="E7" s="2">
+        <v>4.21</v>
+      </c>
+      <c r="F7" s="5">
+        <v>6.7220000000000004</v>
+      </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
@@ -627,6 +657,9 @@
       <c r="E8" s="5">
         <v>4.7667000000000002</v>
       </c>
+      <c r="F8" s="5">
+        <v>8.8733799999999992</v>
+      </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
@@ -644,6 +677,9 @@
       <c r="E9" s="2">
         <v>8.24</v>
       </c>
+      <c r="F9" s="2">
+        <v>13.44</v>
+      </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
@@ -658,6 +694,12 @@
       <c r="D10" s="3">
         <v>9.4600000000000009</v>
       </c>
+      <c r="E10" s="2">
+        <v>9.4600000000000009</v>
+      </c>
+      <c r="F10" s="2">
+        <v>9.4600000000000009</v>
+      </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
@@ -672,6 +714,12 @@
       <c r="D11" s="3">
         <v>27.85</v>
       </c>
+      <c r="E11" s="2">
+        <v>27.85</v>
+      </c>
+      <c r="F11" s="2">
+        <v>27.85</v>
+      </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
@@ -687,7 +735,10 @@
         <v>7.95</v>
       </c>
       <c r="E12" s="5">
-        <v>1.9869000000000001</v>
+        <v>7.95</v>
+      </c>
+      <c r="F12" s="5">
+        <v>7.95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>